<commit_message>
Included comments and documentation
</commit_message>
<xml_diff>
--- a/Aldo-Test-Data1.xlsx
+++ b/Aldo-Test-Data1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hari4\python-webui-filter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CB3E51-4923-4B1A-A5E9-0B9B9BA20DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0996C96-8E95-4850-8AA0-0A43A4833349}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{EDF5FB46-B36E-40B2-AB95-F94766D28BEB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EDF5FB46-B36E-40B2-AB95-F94766D28BEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Filter" sheetId="1" r:id="rId1"/>
@@ -526,7 +526,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +698,7 @@
         <v>35</v>
       </c>
       <c r="M4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -752,21 +752,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F65BFE220852654A94B0E24FAB8D414F" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bdacad30f1d04398aad8d480b298e327">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b7a2423e-e457-463e-bb09-ea35f27c79d5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d7967f50696128c4f60bd15feea58994" ns3:_="">
     <xsd:import namespace="b7a2423e-e457-463e-bb09-ea35f27c79d5"/>
@@ -936,24 +921,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26CAAAA5-B919-4882-8B55-7BA28EC43444}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04331AB7-27E2-427E-B974-CFD943DB3B3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FF27198-C35E-49FE-AC2C-C7F5925F492B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -969,4 +952,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04331AB7-27E2-427E-B974-CFD943DB3B3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26CAAAA5-B919-4882-8B55-7BA28EC43444}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>